<commit_message>
script works for 2022-03
</commit_message>
<xml_diff>
--- a/Q3/Vorplan/Vorplan Plan Q3-22 v4 - Für die Trainer.xlsx
+++ b/Q3/Vorplan/Vorplan Plan Q3-22 v4 - Für die Trainer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MMS\Python\DAV_Quartal\Q3\Vorplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E481068-F16A-4985-AA67-8C33A0C41855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A6C9AD-86E7-4547-837F-13E9521E82C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorplan Q2-22" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Termin 2</t>
-  </si>
-  <si>
-    <t>Termion 3</t>
   </si>
   <si>
     <t>Termin 4</t>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Termin 3</t>
   </si>
 </sst>
 </file>
@@ -791,7 +791,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Zeit"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Termin 1" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Termin 2" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Termion 3" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Termin 3" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Termin 4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1047,23 +1047,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="1"/>
-    <col min="4" max="4" width="11.7265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="11.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="29" style="1" customWidth="1"/>
-    <col min="6" max="10" width="12.54296875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="2.7265625" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="6" max="10" width="12.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" s="1" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:31" s="1" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="2"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1071,10 +1071,10 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="AE1" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
@@ -1087,8 +1087,8 @@
       <c r="I2" s="52"/>
       <c r="J2" s="52"/>
     </row>
-    <row r="3" spans="2:31" ht="10" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:31" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1111,75 +1111,75 @@
         <v>7</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="L4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="Z4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AA4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AB4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AC4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AD4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AE4" s="8" t="s">
+    </row>
+    <row r="5" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="C5" s="10">
         <v>44477</v>
@@ -1188,7 +1188,7 @@
         <v>44743</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -1216,9 +1216,9 @@
       <c r="AD5" s="8"/>
       <c r="AE5" s="8"/>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="10">
         <v>44471</v>
@@ -1227,10 +1227,10 @@
         <v>44744</v>
       </c>
       <c r="E6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>33</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="G6" s="11">
         <v>44744</v>
@@ -1261,17 +1261,17 @@
       <c r="AD6" s="8"/>
       <c r="AE6" s="8"/>
     </row>
-    <row r="7" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="11">
         <v>44744</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="G7" s="11">
         <v>44744</v>
@@ -1302,17 +1302,17 @@
       <c r="AD7" s="8"/>
       <c r="AE7" s="8"/>
     </row>
-    <row r="8" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11">
         <v>44744</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>38</v>
       </c>
       <c r="G8" s="11">
         <v>44744</v>
@@ -1341,9 +1341,9 @@
       <c r="AD8" s="8"/>
       <c r="AE8" s="8"/>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="10">
         <v>44472</v>
@@ -1352,10 +1352,10 @@
         <v>44745</v>
       </c>
       <c r="E9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G9" s="11">
         <v>44745</v>
@@ -1384,17 +1384,17 @@
       <c r="AD9" s="8"/>
       <c r="AE9" s="8"/>
     </row>
-    <row r="10" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11">
         <v>44745</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="11">
         <v>44745</v>
@@ -1423,14 +1423,14 @@
       <c r="AD10" s="8"/>
       <c r="AE10" s="8"/>
     </row>
-    <row r="11" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="11">
         <v>44745</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -1458,9 +1458,9 @@
       <c r="AD11" s="8"/>
       <c r="AE11" s="8"/>
     </row>
-    <row r="12" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="10">
         <v>44473</v>
@@ -1469,10 +1469,10 @@
         <v>44746</v>
       </c>
       <c r="E12" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>44</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>45</v>
       </c>
       <c r="G12" s="11">
         <v>44746</v>
@@ -1484,12 +1484,12 @@
       <c r="J12" s="22"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
@@ -1507,9 +1507,9 @@
       <c r="AD12" s="8"/>
       <c r="AE12" s="8"/>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="10">
         <v>44474</v>
@@ -1518,10 +1518,10 @@
         <v>44747</v>
       </c>
       <c r="E13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G13" s="11">
         <v>44747</v>
@@ -1550,9 +1550,9 @@
       <c r="AD13" s="8"/>
       <c r="AE13" s="8"/>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="10">
         <v>44475</v>
@@ -1561,10 +1561,10 @@
         <v>44748</v>
       </c>
       <c r="E14" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>48</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>49</v>
       </c>
       <c r="G14" s="11">
         <v>44748</v>
@@ -1599,9 +1599,9 @@
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
     </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="10">
         <v>44476</v>
@@ -1610,10 +1610,10 @@
         <v>44749</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="11">
         <v>44749</v>
@@ -1642,9 +1642,9 @@
       <c r="AD15" s="8"/>
       <c r="AE15" s="8"/>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="10">
         <v>44477</v>
@@ -1653,10 +1653,10 @@
         <v>44750</v>
       </c>
       <c r="E16" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="G16" s="11">
         <v>44750</v>
@@ -1671,7 +1671,7 @@
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
@@ -1687,9 +1687,9 @@
       <c r="AD16" s="8"/>
       <c r="AE16" s="8"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="10">
         <v>44471</v>
@@ -1698,10 +1698,10 @@
         <v>44751</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" s="11">
         <v>44751</v>
@@ -1718,7 +1718,7 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
@@ -1734,17 +1734,17 @@
       <c r="AD17" s="8"/>
       <c r="AE17" s="8"/>
     </row>
-    <row r="18" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11">
         <v>44751</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G18" s="11">
         <v>44751</v>
@@ -1775,9 +1775,9 @@
       <c r="AD18" s="8"/>
       <c r="AE18" s="8"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="10">
         <v>44472</v>
@@ -1786,10 +1786,10 @@
         <v>44752</v>
       </c>
       <c r="E19" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G19" s="11">
         <v>44752</v>
@@ -1818,17 +1818,17 @@
       <c r="AD19" s="8"/>
       <c r="AE19" s="8"/>
     </row>
-    <row r="20" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="11">
         <v>44752</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G20" s="11">
         <v>44752</v>
@@ -1857,14 +1857,14 @@
       <c r="AD20" s="8"/>
       <c r="AE20" s="8"/>
     </row>
-    <row r="21" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="11">
         <v>44752</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -1892,9 +1892,9 @@
       <c r="AD21" s="8"/>
       <c r="AE21" s="8"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="10">
         <v>44473</v>
@@ -1903,7 +1903,7 @@
         <v>44753</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
@@ -1931,9 +1931,9 @@
       <c r="AD22" s="8"/>
       <c r="AE22" s="8"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="10">
         <v>44474</v>
@@ -1942,10 +1942,10 @@
         <v>44754</v>
       </c>
       <c r="E23" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G23" s="11">
         <v>44754</v>
@@ -1957,7 +1957,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
@@ -1976,9 +1976,9 @@
       <c r="AD23" s="8"/>
       <c r="AE23" s="8"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="10">
         <v>44475</v>
@@ -1987,7 +1987,7 @@
         <v>44755</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -2015,10 +2015,10 @@
       <c r="AD24" s="8"/>
       <c r="AE24" s="8"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="10">
         <v>44476</v>
@@ -2027,10 +2027,10 @@
         <v>44756</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G25" s="11">
         <v>44756</v>
@@ -2059,10 +2059,10 @@
       <c r="AD25" s="8"/>
       <c r="AE25" s="8"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
       <c r="B26" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="38">
         <v>44477</v>
@@ -2071,10 +2071,10 @@
         <v>44757</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G26" s="11">
         <v>44757</v>
@@ -2087,7 +2087,7 @@
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
@@ -2105,10 +2105,10 @@
       <c r="AD26" s="8"/>
       <c r="AE26" s="8"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
       <c r="B27" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="38">
         <v>44471</v>
@@ -2117,10 +2117,10 @@
         <v>44758</v>
       </c>
       <c r="E27" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="33" t="s">
         <v>33</v>
-      </c>
-      <c r="F27" s="33" t="s">
-        <v>34</v>
       </c>
       <c r="G27" s="11">
         <v>44758</v>
@@ -2134,7 +2134,7 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
@@ -2153,7 +2153,7 @@
       <c r="AD27" s="8"/>
       <c r="AE27" s="8"/>
     </row>
-    <row r="28" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
       <c r="B28" s="37"/>
       <c r="C28" s="38"/>
@@ -2161,10 +2161,10 @@
         <v>44758</v>
       </c>
       <c r="E28" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="39" t="s">
         <v>35</v>
-      </c>
-      <c r="F28" s="39" t="s">
-        <v>36</v>
       </c>
       <c r="G28" s="11">
         <v>44758</v>
@@ -2176,11 +2176,11 @@
       <c r="J28" s="36"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N28" s="8"/>
       <c r="O28" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
@@ -2199,7 +2199,7 @@
       <c r="AD28" s="8"/>
       <c r="AE28" s="8"/>
     </row>
-    <row r="29" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34"/>
       <c r="B29" s="37"/>
       <c r="C29" s="38"/>
@@ -2207,10 +2207,10 @@
         <v>44758</v>
       </c>
       <c r="E29" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="33" t="s">
         <v>37</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>38</v>
       </c>
       <c r="G29" s="11">
         <v>44758</v>
@@ -2239,10 +2239,10 @@
       <c r="AD29" s="8"/>
       <c r="AE29" s="8"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="34"/>
       <c r="B30" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="38">
         <v>44472</v>
@@ -2251,10 +2251,10 @@
         <v>44759</v>
       </c>
       <c r="E30" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G30" s="11">
         <v>44759</v>
@@ -2283,7 +2283,7 @@
       <c r="AD30" s="8"/>
       <c r="AE30" s="8"/>
     </row>
-    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
       <c r="B31" s="37"/>
       <c r="C31" s="38"/>
@@ -2291,10 +2291,10 @@
         <v>44759</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G31" s="11">
         <v>44759</v>
@@ -2323,7 +2323,7 @@
       <c r="AD31" s="8"/>
       <c r="AE31" s="8"/>
     </row>
-    <row r="32" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
       <c r="B32" s="37"/>
       <c r="C32" s="38"/>
@@ -2331,7 +2331,7 @@
         <v>44759</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
@@ -2359,10 +2359,10 @@
       <c r="AD32" s="8"/>
       <c r="AE32" s="8"/>
     </row>
-    <row r="33" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="34"/>
       <c r="B33" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="38">
         <v>44473</v>
@@ -2371,10 +2371,10 @@
         <v>44760</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G33" s="11">
         <v>44760</v>
@@ -2387,7 +2387,7 @@
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
       <c r="P33" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
@@ -2405,10 +2405,10 @@
       <c r="AD33" s="8"/>
       <c r="AE33" s="8"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
       <c r="B34" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34" s="38">
         <v>44474</v>
@@ -2417,10 +2417,10 @@
         <v>44761</v>
       </c>
       <c r="E34" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F34" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G34" s="11">
         <v>44761</v>
@@ -2432,7 +2432,7 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P34" s="8"/>
       <c r="Q34" s="8"/>
@@ -2451,10 +2451,10 @@
       <c r="AD34" s="8"/>
       <c r="AE34" s="8"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="10">
         <v>44475</v>
@@ -2463,7 +2463,7 @@
         <v>44762</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
@@ -2491,10 +2491,10 @@
       <c r="AD35" s="8"/>
       <c r="AE35" s="8"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="34"/>
       <c r="B36" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" s="10">
         <v>44476</v>
@@ -2503,10 +2503,10 @@
         <v>44763</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G36" s="11">
         <v>44763</v>
@@ -2515,7 +2515,7 @@
       <c r="I36" s="21"/>
       <c r="J36" s="22"/>
       <c r="L36" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
@@ -2537,10 +2537,10 @@
       <c r="AD36" s="8"/>
       <c r="AE36" s="8"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="34"/>
       <c r="B37" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="10">
         <v>44477</v>
@@ -2549,10 +2549,10 @@
         <v>44764</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G37" s="11">
         <v>44764</v>
@@ -2566,7 +2566,7 @@
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P37" s="8"/>
       <c r="Q37" s="8"/>
@@ -2585,10 +2585,10 @@
       <c r="AD37" s="8"/>
       <c r="AE37" s="8"/>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="34"/>
       <c r="B38" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="10">
         <v>44471</v>
@@ -2597,10 +2597,10 @@
         <v>44765</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F38" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G38" s="11">
         <v>44765</v>
@@ -2612,14 +2612,14 @@
       <c r="J38" s="22"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N38" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="N38" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="O38" s="8"/>
       <c r="P38" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
@@ -2637,7 +2637,7 @@
       <c r="AD38" s="8"/>
       <c r="AE38" s="8"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10"/>
@@ -2645,10 +2645,10 @@
         <v>44765</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G39" s="11">
         <v>44765</v>
@@ -2659,7 +2659,7 @@
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
@@ -2679,10 +2679,10 @@
       <c r="AD39" s="8"/>
       <c r="AE39" s="8"/>
     </row>
-    <row r="40" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
       <c r="B40" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="10">
         <v>44472</v>
@@ -2691,10 +2691,10 @@
         <v>44766</v>
       </c>
       <c r="E40" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F40" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G40" s="11">
         <v>44766</v>
@@ -2723,7 +2723,7 @@
       <c r="AD40" s="8"/>
       <c r="AE40" s="8"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="34"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10"/>
@@ -2731,10 +2731,10 @@
         <v>44766</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G41" s="11">
         <v>44766</v>
@@ -2763,7 +2763,7 @@
       <c r="AD41" s="8"/>
       <c r="AE41" s="8"/>
     </row>
-    <row r="42" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34"/>
       <c r="B42" s="9"/>
       <c r="C42" s="10"/>
@@ -2771,7 +2771,7 @@
         <v>44766</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
@@ -2799,10 +2799,10 @@
       <c r="AD42" s="8"/>
       <c r="AE42" s="8"/>
     </row>
-    <row r="43" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="34"/>
       <c r="B43" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="10">
         <v>44473</v>
@@ -2811,7 +2811,7 @@
         <v>44767</v>
       </c>
       <c r="E43" s="40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
@@ -2839,10 +2839,10 @@
       <c r="AD43" s="8"/>
       <c r="AE43" s="8"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="34"/>
       <c r="B44" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="10">
         <v>44474</v>
@@ -2851,10 +2851,10 @@
         <v>44768</v>
       </c>
       <c r="E44" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F44" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G44" s="11">
         <v>44768</v>
@@ -2863,14 +2863,14 @@
       <c r="I44" s="21"/>
       <c r="J44" s="22"/>
       <c r="L44" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N44" s="8"/>
       <c r="O44" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P44" s="8"/>
       <c r="Q44" s="8"/>
@@ -2889,10 +2889,10 @@
       <c r="AD44" s="8"/>
       <c r="AE44" s="8"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="34"/>
       <c r="B45" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C45" s="10">
         <v>44475</v>
@@ -2901,7 +2901,7 @@
         <v>44769</v>
       </c>
       <c r="E45" s="40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
@@ -2929,7 +2929,7 @@
       <c r="AD45" s="8"/>
       <c r="AE45" s="8"/>
     </row>
-    <row r="46" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="34"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10"/>
@@ -2937,7 +2937,7 @@
         <v>44769</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
@@ -2965,10 +2965,10 @@
       <c r="AD46" s="8"/>
       <c r="AE46" s="8"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="34"/>
       <c r="B47" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C47" s="10">
         <v>44476</v>
@@ -2977,10 +2977,10 @@
         <v>44770</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G47" s="11">
         <v>44770</v>
@@ -2989,11 +2989,11 @@
       <c r="I47" s="21"/>
       <c r="J47" s="22"/>
       <c r="L47" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M47" s="8"/>
       <c r="N47" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O47" s="8"/>
       <c r="P47" s="8"/>
@@ -3013,10 +3013,10 @@
       <c r="AD47" s="8"/>
       <c r="AE47" s="8"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="34"/>
       <c r="B48" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C48" s="10">
         <v>44477</v>
@@ -3025,7 +3025,7 @@
         <v>44771</v>
       </c>
       <c r="E48" s="40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F48" s="35"/>
       <c r="G48" s="35"/>
@@ -3053,7 +3053,7 @@
       <c r="AD48" s="8"/>
       <c r="AE48" s="8"/>
     </row>
-    <row r="49" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="34"/>
       <c r="B49" s="9"/>
       <c r="C49" s="10"/>
@@ -3061,7 +3061,7 @@
         <v>44771</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F49" s="35"/>
       <c r="G49" s="35"/>
@@ -3089,10 +3089,10 @@
       <c r="AD49" s="8"/>
       <c r="AE49" s="8"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="34"/>
       <c r="B50" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C50" s="10">
         <v>44471</v>
@@ -3101,7 +3101,7 @@
         <v>44772</v>
       </c>
       <c r="E50" s="40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F50" s="41"/>
       <c r="G50" s="41"/>
@@ -3129,7 +3129,7 @@
       <c r="AD50" s="8"/>
       <c r="AE50" s="8"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="34"/>
       <c r="B51" s="9"/>
       <c r="C51" s="10"/>
@@ -3137,10 +3137,10 @@
         <v>44772</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G51" s="11">
         <v>44772</v>
@@ -3153,10 +3153,10 @@
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
       <c r="N51" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O51" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="O51" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="P51" s="8"/>
       <c r="Q51" s="8"/>
@@ -3175,7 +3175,7 @@
       <c r="AD51" s="8"/>
       <c r="AE51" s="8"/>
     </row>
-    <row r="52" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="34"/>
       <c r="B52" s="9"/>
       <c r="C52" s="10"/>
@@ -3183,10 +3183,10 @@
         <v>44772</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F52" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G52" s="11">
         <v>44772</v>
@@ -3217,10 +3217,10 @@
       <c r="AD52" s="8"/>
       <c r="AE52" s="8"/>
     </row>
-    <row r="53" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="34"/>
       <c r="B53" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C53" s="38">
         <v>44472</v>
@@ -3229,10 +3229,10 @@
         <v>44773</v>
       </c>
       <c r="E53" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="35" t="s">
         <v>39</v>
-      </c>
-      <c r="F53" s="35" t="s">
-        <v>40</v>
       </c>
       <c r="G53" s="35"/>
       <c r="H53" s="35"/>
@@ -3241,10 +3241,10 @@
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
       <c r="N53" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O53" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="O53" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="P53" s="8"/>
       <c r="Q53" s="8"/>
@@ -3263,7 +3263,7 @@
       <c r="AD53" s="8"/>
       <c r="AE53" s="8"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="34"/>
       <c r="B54" s="37"/>
       <c r="C54" s="38"/>
@@ -3271,10 +3271,10 @@
         <v>44773</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F54" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G54" s="35"/>
       <c r="H54" s="35"/>
@@ -3283,10 +3283,10 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
       <c r="N54" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O54" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="O54" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="P54" s="8"/>
       <c r="Q54" s="8"/>
@@ -3305,7 +3305,7 @@
       <c r="AD54" s="8"/>
       <c r="AE54" s="8"/>
     </row>
-    <row r="55" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="34"/>
       <c r="B55" s="37"/>
       <c r="C55" s="38"/>
@@ -3313,7 +3313,7 @@
         <v>44773</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
@@ -3341,10 +3341,10 @@
       <c r="AD55" s="8"/>
       <c r="AE55" s="8"/>
     </row>
-    <row r="56" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="34"/>
       <c r="B56" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C56" s="38">
         <v>44473</v>
@@ -3353,10 +3353,10 @@
         <v>44774</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G56" s="11">
         <v>44774</v>
@@ -3391,10 +3391,10 @@
       <c r="AD56" s="8"/>
       <c r="AE56" s="8"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="34"/>
       <c r="B57" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C57" s="10">
         <v>44474</v>
@@ -3403,10 +3403,10 @@
         <v>44775</v>
       </c>
       <c r="E57" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G57" s="11">
         <v>44775</v>
@@ -3415,12 +3415,12 @@
       <c r="I57" s="21"/>
       <c r="J57" s="22"/>
       <c r="L57" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M57" s="8"/>
       <c r="N57" s="8"/>
       <c r="O57" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P57" s="8"/>
       <c r="Q57" s="8"/>
@@ -3439,10 +3439,10 @@
       <c r="AD57" s="8"/>
       <c r="AE57" s="8"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="34"/>
       <c r="B58" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C58" s="10">
         <v>44475</v>
@@ -3451,10 +3451,10 @@
         <v>44776</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G58" s="11">
         <v>44776</v>
@@ -3485,10 +3485,10 @@
       <c r="AD58" s="8"/>
       <c r="AE58" s="8"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="34"/>
       <c r="B59" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C59" s="10">
         <v>44476</v>
@@ -3497,10 +3497,10 @@
         <v>44777</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G59" s="11">
         <v>44777</v>
@@ -3509,7 +3509,7 @@
       <c r="I59" s="21"/>
       <c r="J59" s="22"/>
       <c r="L59" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
@@ -3531,10 +3531,10 @@
       <c r="AD59" s="8"/>
       <c r="AE59" s="8"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="34"/>
       <c r="B60" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C60" s="10">
         <v>44477</v>
@@ -3543,10 +3543,10 @@
         <v>44778</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G60" s="11">
         <v>44778</v>
@@ -3575,10 +3575,10 @@
       <c r="AD60" s="8"/>
       <c r="AE60" s="8"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="34"/>
       <c r="B61" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C61" s="10">
         <v>44471</v>
@@ -3587,10 +3587,10 @@
         <v>44779</v>
       </c>
       <c r="E61" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" s="16" t="s">
         <v>33</v>
-      </c>
-      <c r="F61" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="G61" s="11">
         <v>44779</v>
@@ -3621,7 +3621,7 @@
       <c r="AD61" s="8"/>
       <c r="AE61" s="8"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="34"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
@@ -3629,10 +3629,10 @@
         <v>44779</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G62" s="11">
         <v>44779</v>
@@ -3644,7 +3644,7 @@
       <c r="J62" s="32"/>
       <c r="L62" s="8"/>
       <c r="M62" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N62" s="8"/>
       <c r="O62" s="8"/>
@@ -3665,10 +3665,10 @@
       <c r="AD62" s="8"/>
       <c r="AE62" s="8"/>
     </row>
-    <row r="63" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="34"/>
       <c r="B63" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C63" s="10">
         <v>44472</v>
@@ -3677,10 +3677,10 @@
         <v>44780</v>
       </c>
       <c r="E63" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F63" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G63" s="11">
         <v>44780</v>
@@ -3709,7 +3709,7 @@
       <c r="AD63" s="8"/>
       <c r="AE63" s="8"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" s="34"/>
       <c r="B64" s="9"/>
       <c r="C64" s="10"/>
@@ -3717,10 +3717,10 @@
         <v>44780</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G64" s="11">
         <v>44780</v>
@@ -3749,7 +3749,7 @@
       <c r="AD64" s="8"/>
       <c r="AE64" s="8"/>
     </row>
-    <row r="65" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="34"/>
       <c r="B65" s="9"/>
       <c r="C65" s="10"/>
@@ -3757,7 +3757,7 @@
         <v>44780</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
@@ -3785,10 +3785,10 @@
       <c r="AD65" s="8"/>
       <c r="AE65" s="8"/>
     </row>
-    <row r="66" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="34"/>
       <c r="B66" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C66" s="10">
         <v>44473</v>
@@ -3797,7 +3797,7 @@
         <v>44781</v>
       </c>
       <c r="E66" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F66" s="21"/>
       <c r="G66" s="21"/>
@@ -3825,10 +3825,10 @@
       <c r="AD66" s="8"/>
       <c r="AE66" s="8"/>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" s="34"/>
       <c r="B67" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C67" s="10">
         <v>44474</v>
@@ -3837,10 +3837,10 @@
         <v>44782</v>
       </c>
       <c r="E67" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F67" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F67" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G67" s="11">
         <v>44782</v>
@@ -3869,10 +3869,10 @@
       <c r="AD67" s="8"/>
       <c r="AE67" s="8"/>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" s="34"/>
       <c r="B68" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C68" s="10">
         <v>44475</v>
@@ -3881,7 +3881,7 @@
         <v>44783</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
@@ -3909,10 +3909,10 @@
       <c r="AD68" s="8"/>
       <c r="AE68" s="8"/>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" s="34"/>
       <c r="B69" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C69" s="10">
         <v>44476</v>
@@ -3921,10 +3921,10 @@
         <v>44784</v>
       </c>
       <c r="E69" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G69" s="11">
         <v>44784</v>
@@ -3935,7 +3935,7 @@
       <c r="L69" s="8"/>
       <c r="M69" s="8"/>
       <c r="N69" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O69" s="8"/>
       <c r="P69" s="8"/>
@@ -3955,10 +3955,10 @@
       <c r="AD69" s="8"/>
       <c r="AE69" s="8"/>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" s="34"/>
       <c r="B70" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C70" s="10">
         <v>44477</v>
@@ -3967,10 +3967,10 @@
         <v>44785</v>
       </c>
       <c r="E70" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G70" s="11">
         <v>44785</v>
@@ -4005,10 +4005,10 @@
       <c r="AD70" s="8"/>
       <c r="AE70" s="8"/>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" s="34"/>
       <c r="B71" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C71" s="10">
         <v>44471</v>
@@ -4017,10 +4017,10 @@
         <v>44786</v>
       </c>
       <c r="E71" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F71" s="16" t="s">
         <v>33</v>
-      </c>
-      <c r="F71" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="G71" s="11">
         <v>44786</v>
@@ -4033,7 +4033,7 @@
       <c r="L71" s="8"/>
       <c r="M71" s="8"/>
       <c r="N71" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O71" s="8"/>
       <c r="P71" s="8"/>
@@ -4053,7 +4053,7 @@
       <c r="AD71" s="8"/>
       <c r="AE71" s="8"/>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A72" s="34"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
@@ -4061,10 +4061,10 @@
         <v>44786</v>
       </c>
       <c r="E72" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F72" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="F72" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="G72" s="11">
         <v>44786</v>
@@ -4077,7 +4077,7 @@
       <c r="L72" s="8"/>
       <c r="M72" s="8"/>
       <c r="N72" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O72" s="8"/>
       <c r="P72" s="8"/>
@@ -4097,7 +4097,7 @@
       <c r="AD72" s="8"/>
       <c r="AE72" s="8"/>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" s="34"/>
       <c r="B73" s="9"/>
       <c r="C73" s="10"/>
@@ -4105,10 +4105,10 @@
         <v>44786</v>
       </c>
       <c r="E73" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F73" s="41" t="s">
         <v>50</v>
-      </c>
-      <c r="F73" s="41" t="s">
-        <v>51</v>
       </c>
       <c r="G73" s="11">
         <v>44786</v>
@@ -4137,10 +4137,10 @@
       <c r="AD73" s="8"/>
       <c r="AE73" s="8"/>
     </row>
-    <row r="74" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="34"/>
       <c r="B74" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C74" s="10">
         <v>44472</v>
@@ -4149,10 +4149,10 @@
         <v>44787</v>
       </c>
       <c r="E74" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F74" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G74" s="11">
         <v>44787</v>
@@ -4181,7 +4181,7 @@
       <c r="AD74" s="8"/>
       <c r="AE74" s="8"/>
     </row>
-    <row r="75" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="34"/>
       <c r="B75" s="9"/>
       <c r="C75" s="10"/>
@@ -4189,10 +4189,10 @@
         <v>44787</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F75" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G75" s="11">
         <v>44787</v>
@@ -4221,7 +4221,7 @@
       <c r="AD75" s="8"/>
       <c r="AE75" s="8"/>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76" s="34"/>
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
@@ -4229,7 +4229,7 @@
         <v>44787</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
@@ -4257,10 +4257,10 @@
       <c r="AD76" s="8"/>
       <c r="AE76" s="8"/>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A77" s="34"/>
       <c r="B77" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C77" s="10">
         <v>44473</v>
@@ -4269,7 +4269,7 @@
         <v>44788</v>
       </c>
       <c r="E77" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F77" s="21"/>
       <c r="G77" s="21"/>
@@ -4297,10 +4297,10 @@
       <c r="AD77" s="8"/>
       <c r="AE77" s="8"/>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A78" s="34"/>
       <c r="B78" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C78" s="10">
         <v>44474</v>
@@ -4309,10 +4309,10 @@
         <v>44789</v>
       </c>
       <c r="E78" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F78" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F78" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G78" s="11">
         <v>44789</v>
@@ -4324,7 +4324,7 @@
       <c r="M78" s="8"/>
       <c r="N78" s="8"/>
       <c r="O78" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P78" s="8"/>
       <c r="Q78" s="8"/>
@@ -4343,10 +4343,10 @@
       <c r="AD78" s="8"/>
       <c r="AE78" s="8"/>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A79" s="34"/>
       <c r="B79" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C79" s="10">
         <v>44475</v>
@@ -4355,10 +4355,10 @@
         <v>44790</v>
       </c>
       <c r="E79" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F79" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="G79" s="11">
         <v>44790</v>
@@ -4389,10 +4389,10 @@
       <c r="AD79" s="8"/>
       <c r="AE79" s="8"/>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A80" s="34"/>
       <c r="B80" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C80" s="10">
         <v>44476</v>
@@ -4401,10 +4401,10 @@
         <v>44791</v>
       </c>
       <c r="E80" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F80" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G80" s="11">
         <v>44791</v>
@@ -4433,10 +4433,10 @@
       <c r="AD80" s="8"/>
       <c r="AE80" s="8"/>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A81" s="34"/>
       <c r="B81" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C81" s="10">
         <v>44477</v>
@@ -4445,7 +4445,7 @@
         <v>44792</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F81" s="13"/>
       <c r="G81" s="13"/>
@@ -4473,10 +4473,10 @@
       <c r="AD81" s="8"/>
       <c r="AE81" s="8"/>
     </row>
-    <row r="82" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="34"/>
       <c r="B82" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C82" s="10">
         <v>44471</v>
@@ -4485,10 +4485,10 @@
         <v>44793</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F82" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G82" s="11">
         <v>44793</v>
@@ -4519,7 +4519,7 @@
       <c r="AD82" s="8"/>
       <c r="AE82" s="8"/>
     </row>
-    <row r="83" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="34"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
@@ -4527,10 +4527,10 @@
         <v>44793</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F83" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G83" s="11">
         <v>44793</v>
@@ -4561,7 +4561,7 @@
       <c r="AD83" s="8"/>
       <c r="AE83" s="8"/>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A84" s="34"/>
       <c r="B84" s="9"/>
       <c r="C84" s="10"/>
@@ -4569,10 +4569,10 @@
         <v>44793</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F84" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G84" s="11">
         <v>44793</v>
@@ -4601,10 +4601,10 @@
       <c r="AD84" s="8"/>
       <c r="AE84" s="8"/>
     </row>
-    <row r="85" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="34"/>
       <c r="B85" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C85" s="10">
         <v>44472</v>
@@ -4613,10 +4613,10 @@
         <v>44794</v>
       </c>
       <c r="E85" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F85" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F85" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G85" s="11">
         <v>44794</v>
@@ -4645,7 +4645,7 @@
       <c r="AD85" s="8"/>
       <c r="AE85" s="8"/>
     </row>
-    <row r="86" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="34"/>
       <c r="B86" s="9"/>
       <c r="C86" s="10"/>
@@ -4653,10 +4653,10 @@
         <v>44794</v>
       </c>
       <c r="E86" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G86" s="11">
         <v>44794</v>
@@ -4685,7 +4685,7 @@
       <c r="AD86" s="8"/>
       <c r="AE86" s="8"/>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A87" s="34"/>
       <c r="B87" s="9"/>
       <c r="C87" s="10"/>
@@ -4693,7 +4693,7 @@
         <v>44794</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F87" s="13"/>
       <c r="G87" s="13"/>
@@ -4721,10 +4721,10 @@
       <c r="AD87" s="8"/>
       <c r="AE87" s="8"/>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A88" s="34"/>
       <c r="B88" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C88" s="10">
         <v>44473</v>
@@ -4733,7 +4733,7 @@
         <v>44795</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F88" s="13"/>
       <c r="G88" s="13"/>
@@ -4761,10 +4761,10 @@
       <c r="AD88" s="8"/>
       <c r="AE88" s="8"/>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A89" s="34"/>
       <c r="B89" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C89" s="10">
         <v>44474</v>
@@ -4773,10 +4773,10 @@
         <v>44796</v>
       </c>
       <c r="E89" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F89" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G89" s="11">
         <v>44796</v>
@@ -4805,10 +4805,10 @@
       <c r="AD89" s="8"/>
       <c r="AE89" s="8"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A90" s="34"/>
       <c r="B90" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C90" s="10">
         <v>44475</v>
@@ -4817,10 +4817,10 @@
         <v>44797</v>
       </c>
       <c r="E90" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F90" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G90" s="11">
         <v>44797</v>
@@ -4849,9 +4849,9 @@
       <c r="AD90" s="8"/>
       <c r="AE90" s="8"/>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B91" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C91" s="38">
         <v>44476</v>
@@ -4860,10 +4860,10 @@
         <v>44798</v>
       </c>
       <c r="E91" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F91" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G91" s="11">
         <v>44798</v>
@@ -4874,7 +4874,7 @@
       <c r="L91" s="8"/>
       <c r="M91" s="8"/>
       <c r="N91" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O91" s="8"/>
       <c r="P91" s="8"/>
@@ -4894,9 +4894,9 @@
       <c r="AD91" s="8"/>
       <c r="AE91" s="8"/>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B92" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C92" s="10">
         <v>44477</v>
@@ -4905,7 +4905,7 @@
         <v>44799</v>
       </c>
       <c r="E92" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F92" s="13"/>
       <c r="G92" s="13"/>
@@ -4933,9 +4933,9 @@
       <c r="AD92" s="8"/>
       <c r="AE92" s="8"/>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B93" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C93" s="10">
         <v>44471</v>
@@ -4944,10 +4944,10 @@
         <v>44800</v>
       </c>
       <c r="E93" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F93" s="33" t="s">
         <v>33</v>
-      </c>
-      <c r="F93" s="33" t="s">
-        <v>34</v>
       </c>
       <c r="G93" s="11">
         <v>44800</v>
@@ -4960,10 +4960,10 @@
       <c r="L93" s="8"/>
       <c r="M93" s="8"/>
       <c r="N93" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O93" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="O93" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="P93" s="8"/>
       <c r="Q93" s="8"/>
@@ -4982,17 +4982,17 @@
       <c r="AD93" s="8"/>
       <c r="AE93" s="8"/>
     </row>
-    <row r="94" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
       <c r="D94" s="11">
         <v>44800</v>
       </c>
       <c r="E94" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F94" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="F94" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="G94" s="11">
         <v>44800</v>
@@ -5005,10 +5005,10 @@
       <c r="L94" s="8"/>
       <c r="M94" s="8"/>
       <c r="N94" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O94" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="O94" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="P94" s="8"/>
       <c r="Q94" s="8"/>
@@ -5027,17 +5027,17 @@
       <c r="AD94" s="8"/>
       <c r="AE94" s="8"/>
     </row>
-    <row r="95" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
       <c r="D95" s="11">
         <v>44800</v>
       </c>
       <c r="E95" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F95" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="F95" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="G95" s="11">
         <v>44800</v>
@@ -5048,10 +5048,10 @@
       <c r="L95" s="8"/>
       <c r="M95" s="8"/>
       <c r="N95" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O95" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="O95" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="P95" s="8"/>
       <c r="Q95" s="8"/>
@@ -5070,9 +5070,9 @@
       <c r="AD95" s="8"/>
       <c r="AE95" s="8"/>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B96" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C96" s="10">
         <v>44472</v>
@@ -5081,10 +5081,10 @@
         <v>44801</v>
       </c>
       <c r="E96" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F96" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F96" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G96" s="11">
         <v>44801</v>
@@ -5113,17 +5113,17 @@
       <c r="AD96" s="8"/>
       <c r="AE96" s="8"/>
     </row>
-    <row r="97" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
       <c r="D97" s="11">
         <v>44801</v>
       </c>
       <c r="E97" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G97" s="11">
         <v>44801</v>
@@ -5152,14 +5152,14 @@
       <c r="AD97" s="8"/>
       <c r="AE97" s="8"/>
     </row>
-    <row r="98" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
       <c r="D98" s="11">
         <v>44801</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F98" s="13"/>
       <c r="G98" s="13"/>
@@ -5187,9 +5187,9 @@
       <c r="AD98" s="8"/>
       <c r="AE98" s="8"/>
     </row>
-    <row r="99" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B99" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C99" s="10">
         <v>44473</v>
@@ -5198,10 +5198,10 @@
         <v>44802</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G99" s="11">
         <v>44802</v>
@@ -5215,7 +5215,7 @@
       <c r="M99" s="8"/>
       <c r="N99" s="8"/>
       <c r="O99" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P99" s="8"/>
       <c r="Q99" s="8"/>
@@ -5234,9 +5234,9 @@
       <c r="AD99" s="8"/>
       <c r="AE99" s="8"/>
     </row>
-    <row r="100" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B100" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C100" s="10">
         <v>44474</v>
@@ -5245,10 +5245,10 @@
         <v>44803</v>
       </c>
       <c r="E100" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F100" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F100" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G100" s="11">
         <v>44803</v>
@@ -5260,7 +5260,7 @@
       <c r="M100" s="8"/>
       <c r="N100" s="8"/>
       <c r="O100" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P100" s="8"/>
       <c r="Q100" s="8"/>
@@ -5279,9 +5279,9 @@
       <c r="AD100" s="8"/>
       <c r="AE100" s="8"/>
     </row>
-    <row r="101" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C101" s="10">
         <v>44475</v>
@@ -5290,7 +5290,7 @@
         <v>44804</v>
       </c>
       <c r="E101" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F101" s="13"/>
       <c r="G101" s="13"/>
@@ -5318,9 +5318,9 @@
       <c r="AD101" s="8"/>
       <c r="AE101" s="8"/>
     </row>
-    <row r="102" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B102" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C102" s="10">
         <v>44476</v>
@@ -5329,10 +5329,10 @@
         <v>44805</v>
       </c>
       <c r="E102" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F102" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G102" s="11">
         <v>44805</v>
@@ -5361,9 +5361,9 @@
       <c r="AD102" s="8"/>
       <c r="AE102" s="8"/>
     </row>
-    <row r="103" spans="2:31" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:31" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C103" s="10">
         <v>44477</v>
@@ -5372,7 +5372,7 @@
         <v>44806</v>
       </c>
       <c r="E103" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F103" s="13"/>
       <c r="G103" s="13"/>
@@ -5400,9 +5400,9 @@
       <c r="AD103" s="8"/>
       <c r="AE103" s="8"/>
     </row>
-    <row r="104" spans="2:31" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:31" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C104" s="10">
         <v>44471</v>
@@ -5411,7 +5411,7 @@
         <v>44807</v>
       </c>
       <c r="E104" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F104" s="13"/>
       <c r="G104" s="13"/>
@@ -5439,17 +5439,17 @@
       <c r="AD104" s="8"/>
       <c r="AE104" s="8"/>
     </row>
-    <row r="105" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="9"/>
       <c r="C105" s="10"/>
       <c r="D105" s="11">
         <v>44807</v>
       </c>
       <c r="E105" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F105" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="F105" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="G105" s="11">
         <v>44807</v>
@@ -5463,7 +5463,7 @@
       <c r="M105" s="8"/>
       <c r="N105" s="8"/>
       <c r="O105" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P105" s="8"/>
       <c r="Q105" s="8"/>
@@ -5482,17 +5482,17 @@
       <c r="AD105" s="8"/>
       <c r="AE105" s="8"/>
     </row>
-    <row r="106" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B106" s="9"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11">
         <v>44807</v>
       </c>
       <c r="E106" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F106" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="F106" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="G106" s="11">
         <v>44807</v>
@@ -5521,9 +5521,9 @@
       <c r="AD106" s="8"/>
       <c r="AE106" s="8"/>
     </row>
-    <row r="107" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C107" s="38">
         <v>44472</v>
@@ -5532,7 +5532,7 @@
         <v>44808</v>
       </c>
       <c r="E107" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F107" s="21"/>
       <c r="G107" s="21"/>
@@ -5560,17 +5560,17 @@
       <c r="AD107" s="8"/>
       <c r="AE107" s="8"/>
     </row>
-    <row r="108" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B108" s="37"/>
       <c r="C108" s="38"/>
       <c r="D108" s="11">
         <v>44808</v>
       </c>
       <c r="E108" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F108" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F108" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G108" s="11">
         <v>44808</v>
@@ -5582,7 +5582,7 @@
       <c r="M108" s="8"/>
       <c r="N108" s="8"/>
       <c r="O108" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P108" s="8"/>
       <c r="Q108" s="8"/>
@@ -5601,17 +5601,17 @@
       <c r="AD108" s="8"/>
       <c r="AE108" s="8"/>
     </row>
-    <row r="109" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="37"/>
       <c r="C109" s="38"/>
       <c r="D109" s="11">
         <v>44808</v>
       </c>
       <c r="E109" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F109" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G109" s="11">
         <v>44808</v>
@@ -5623,7 +5623,7 @@
       <c r="M109" s="8"/>
       <c r="N109" s="8"/>
       <c r="O109" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P109" s="8"/>
       <c r="Q109" s="8"/>
@@ -5642,14 +5642,14 @@
       <c r="AD109" s="8"/>
       <c r="AE109" s="8"/>
     </row>
-    <row r="110" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="37"/>
       <c r="C110" s="38"/>
       <c r="D110" s="11">
         <v>44808</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F110" s="13"/>
       <c r="G110" s="13"/>
@@ -5677,9 +5677,9 @@
       <c r="AD110" s="8"/>
       <c r="AE110" s="8"/>
     </row>
-    <row r="111" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B111" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C111" s="38">
         <v>44473</v>
@@ -5688,7 +5688,7 @@
         <v>44809</v>
       </c>
       <c r="E111" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F111" s="13"/>
       <c r="G111" s="13"/>
@@ -5716,9 +5716,9 @@
       <c r="AD111" s="8"/>
       <c r="AE111" s="8"/>
     </row>
-    <row r="112" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B112" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C112" s="10">
         <v>44474</v>
@@ -5727,10 +5727,10 @@
         <v>44810</v>
       </c>
       <c r="E112" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F112" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F112" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G112" s="11">
         <v>44810</v>
@@ -5742,7 +5742,7 @@
       <c r="M112" s="8"/>
       <c r="N112" s="8"/>
       <c r="O112" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P112" s="8"/>
       <c r="Q112" s="8"/>
@@ -5761,9 +5761,9 @@
       <c r="AD112" s="8"/>
       <c r="AE112" s="8"/>
     </row>
-    <row r="113" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B113" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C113" s="10">
         <v>44475</v>
@@ -5772,7 +5772,7 @@
         <v>44811</v>
       </c>
       <c r="E113" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F113" s="31"/>
       <c r="G113" s="11"/>
@@ -5800,9 +5800,9 @@
       <c r="AD113" s="8"/>
       <c r="AE113" s="8"/>
     </row>
-    <row r="114" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B114" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C114" s="10">
         <v>44476</v>
@@ -5811,10 +5811,10 @@
         <v>44812</v>
       </c>
       <c r="E114" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F114" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G114" s="11">
         <v>44812</v>
@@ -5825,7 +5825,7 @@
       <c r="L114" s="8"/>
       <c r="M114" s="8"/>
       <c r="N114" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O114" s="8"/>
       <c r="P114" s="8"/>
@@ -5845,9 +5845,9 @@
       <c r="AD114" s="8"/>
       <c r="AE114" s="8"/>
     </row>
-    <row r="115" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B115" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C115" s="10">
         <v>44477</v>
@@ -5856,10 +5856,10 @@
         <v>44813</v>
       </c>
       <c r="E115" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G115" s="11">
         <v>44813</v>
@@ -5873,7 +5873,7 @@
       <c r="M115" s="8"/>
       <c r="N115" s="8"/>
       <c r="O115" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P115" s="8"/>
       <c r="Q115" s="8"/>
@@ -5892,9 +5892,9 @@
       <c r="AD115" s="8"/>
       <c r="AE115" s="8"/>
     </row>
-    <row r="116" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B116" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C116" s="10">
         <v>44471</v>
@@ -5903,10 +5903,10 @@
         <v>44814</v>
       </c>
       <c r="E116" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G116" s="11">
         <v>44814</v>
@@ -5937,17 +5937,17 @@
       <c r="AD116" s="8"/>
       <c r="AE116" s="8"/>
     </row>
-    <row r="117" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="9"/>
       <c r="C117" s="10"/>
       <c r="D117" s="11">
         <v>44814</v>
       </c>
       <c r="E117" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G117" s="11">
         <v>44814</v>
@@ -5959,7 +5959,7 @@
       <c r="J117" s="14"/>
       <c r="L117" s="8"/>
       <c r="M117" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N117" s="8"/>
       <c r="O117" s="8"/>
@@ -5980,17 +5980,17 @@
       <c r="AD117" s="8"/>
       <c r="AE117" s="8"/>
     </row>
-    <row r="118" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="9"/>
       <c r="C118" s="10"/>
       <c r="D118" s="11">
         <v>44814</v>
       </c>
       <c r="E118" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G118" s="11">
         <v>44814</v>
@@ -6019,9 +6019,9 @@
       <c r="AD118" s="8"/>
       <c r="AE118" s="8"/>
     </row>
-    <row r="119" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B119" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C119" s="10">
         <v>44472</v>
@@ -6030,10 +6030,10 @@
         <v>44815</v>
       </c>
       <c r="E119" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F119" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F119" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G119" s="11">
         <v>44815</v>
@@ -6062,17 +6062,17 @@
       <c r="AD119" s="8"/>
       <c r="AE119" s="8"/>
     </row>
-    <row r="120" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="9"/>
       <c r="C120" s="10"/>
       <c r="D120" s="11">
         <v>44815</v>
       </c>
       <c r="E120" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F120" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G120" s="11">
         <v>44815</v>
@@ -6101,14 +6101,14 @@
       <c r="AD120" s="8"/>
       <c r="AE120" s="8"/>
     </row>
-    <row r="121" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="9"/>
       <c r="C121" s="10"/>
       <c r="D121" s="11">
         <v>44815</v>
       </c>
       <c r="E121" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F121" s="13"/>
       <c r="G121" s="13"/>
@@ -6136,9 +6136,9 @@
       <c r="AD121" s="8"/>
       <c r="AE121" s="8"/>
     </row>
-    <row r="122" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B122" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C122" s="10">
         <v>44473</v>
@@ -6147,10 +6147,10 @@
         <v>44816</v>
       </c>
       <c r="E122" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F122" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G122" s="11">
         <v>44816</v>
@@ -6170,7 +6170,7 @@
       <c r="O122" s="8"/>
       <c r="P122" s="8"/>
       <c r="Q122" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R122" s="8"/>
       <c r="S122" s="8"/>
@@ -6187,9 +6187,9 @@
       <c r="AD122" s="8"/>
       <c r="AE122" s="8"/>
     </row>
-    <row r="123" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B123" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C123" s="10">
         <v>44474</v>
@@ -6198,10 +6198,10 @@
         <v>44817</v>
       </c>
       <c r="E123" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F123" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F123" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G123" s="11">
         <v>44817</v>
@@ -6213,7 +6213,7 @@
       <c r="M123" s="8"/>
       <c r="N123" s="8"/>
       <c r="O123" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P123" s="8"/>
       <c r="Q123" s="8"/>
@@ -6232,9 +6232,9 @@
       <c r="AD123" s="8"/>
       <c r="AE123" s="8"/>
     </row>
-    <row r="124" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B124" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C124" s="10">
         <v>44475</v>
@@ -6243,10 +6243,10 @@
         <v>44818</v>
       </c>
       <c r="E124" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F124" s="41" t="s">
         <v>50</v>
-      </c>
-      <c r="F124" s="41" t="s">
-        <v>51</v>
       </c>
       <c r="G124" s="11">
         <v>44818</v>
@@ -6275,9 +6275,9 @@
       <c r="AD124" s="8"/>
       <c r="AE124" s="8"/>
     </row>
-    <row r="125" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B125" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C125" s="10">
         <v>44476</v>
@@ -6286,10 +6286,10 @@
         <v>44819</v>
       </c>
       <c r="E125" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F125" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G125" s="11">
         <v>44819</v>
@@ -6318,9 +6318,9 @@
       <c r="AD125" s="8"/>
       <c r="AE125" s="8"/>
     </row>
-    <row r="126" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B126" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C126" s="10">
         <v>44477</v>
@@ -6329,7 +6329,7 @@
         <v>44820</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F126" s="13"/>
       <c r="G126" s="13"/>
@@ -6357,9 +6357,9 @@
       <c r="AD126" s="8"/>
       <c r="AE126" s="8"/>
     </row>
-    <row r="127" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B127" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C127" s="10">
         <v>44471</v>
@@ -6368,10 +6368,10 @@
         <v>44821</v>
       </c>
       <c r="E127" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F127" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="F127" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="G127" s="11">
         <v>44821</v>
@@ -6384,7 +6384,7 @@
       <c r="L127" s="8"/>
       <c r="M127" s="8"/>
       <c r="N127" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O127" s="8"/>
       <c r="P127" s="8"/>
@@ -6404,17 +6404,17 @@
       <c r="AD127" s="8"/>
       <c r="AE127" s="8"/>
     </row>
-    <row r="128" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="9"/>
       <c r="C128" s="10"/>
       <c r="D128" s="11">
         <v>44821</v>
       </c>
       <c r="E128" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F128" s="45" t="s">
         <v>35</v>
-      </c>
-      <c r="F128" s="45" t="s">
-        <v>36</v>
       </c>
       <c r="G128" s="11">
         <v>44821</v>
@@ -6426,10 +6426,10 @@
       <c r="J128" s="22"/>
       <c r="L128" s="8"/>
       <c r="M128" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N128" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="N128" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="O128" s="8"/>
       <c r="P128" s="8"/>
@@ -6449,17 +6449,17 @@
       <c r="AD128" s="8"/>
       <c r="AE128" s="8"/>
     </row>
-    <row r="129" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="9"/>
       <c r="C129" s="10"/>
       <c r="D129" s="11">
         <v>44821</v>
       </c>
       <c r="E129" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F129" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="F129" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="G129" s="11">
         <v>44821</v>
@@ -6470,7 +6470,7 @@
       <c r="L129" s="8"/>
       <c r="M129" s="8"/>
       <c r="N129" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O129" s="8"/>
       <c r="P129" s="8"/>
@@ -6490,9 +6490,9 @@
       <c r="AD129" s="8"/>
       <c r="AE129" s="8"/>
     </row>
-    <row r="130" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B130" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C130" s="10">
         <v>44472</v>
@@ -6501,10 +6501,10 @@
         <v>44822</v>
       </c>
       <c r="E130" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F130" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F130" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G130" s="11">
         <v>44822</v>
@@ -6533,17 +6533,17 @@
       <c r="AD130" s="8"/>
       <c r="AE130" s="8"/>
     </row>
-    <row r="131" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B131" s="9"/>
       <c r="C131" s="10"/>
       <c r="D131" s="11">
         <v>44822</v>
       </c>
       <c r="E131" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F131" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G131" s="11">
         <v>44822</v>
@@ -6572,14 +6572,14 @@
       <c r="AD131" s="8"/>
       <c r="AE131" s="8"/>
     </row>
-    <row r="132" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B132" s="9"/>
       <c r="C132" s="10"/>
       <c r="D132" s="11">
         <v>44822</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F132" s="13"/>
       <c r="G132" s="13"/>
@@ -6607,9 +6607,9 @@
       <c r="AD132" s="8"/>
       <c r="AE132" s="8"/>
     </row>
-    <row r="133" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B133" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C133" s="10">
         <v>44473</v>
@@ -6618,7 +6618,7 @@
         <v>44823</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F133" s="13"/>
       <c r="G133" s="13"/>
@@ -6646,9 +6646,9 @@
       <c r="AD133" s="8"/>
       <c r="AE133" s="8"/>
     </row>
-    <row r="134" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B134" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C134" s="10">
         <v>44474</v>
@@ -6657,10 +6657,10 @@
         <v>44824</v>
       </c>
       <c r="E134" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F134" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F134" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G134" s="11">
         <v>44824</v>
@@ -6670,7 +6670,7 @@
       <c r="J134" s="22"/>
       <c r="L134" s="8"/>
       <c r="M134" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N134" s="8"/>
       <c r="O134" s="8"/>
@@ -6691,9 +6691,9 @@
       <c r="AD134" s="8"/>
       <c r="AE134" s="8"/>
     </row>
-    <row r="135" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B135" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C135" s="10">
         <v>44475</v>
@@ -6702,7 +6702,7 @@
         <v>44825</v>
       </c>
       <c r="E135" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F135" s="13"/>
       <c r="G135" s="13"/>
@@ -6730,9 +6730,9 @@
       <c r="AD135" s="8"/>
       <c r="AE135" s="8"/>
     </row>
-    <row r="136" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B136" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C136" s="10">
         <v>44476</v>
@@ -6741,10 +6741,10 @@
         <v>44826</v>
       </c>
       <c r="E136" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F136" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G136" s="11">
         <v>44826</v>
@@ -6755,7 +6755,7 @@
       <c r="L136" s="8"/>
       <c r="M136" s="8"/>
       <c r="N136" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O136" s="8"/>
       <c r="P136" s="8"/>
@@ -6775,9 +6775,9 @@
       <c r="AD136" s="8"/>
       <c r="AE136" s="8"/>
     </row>
-    <row r="137" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B137" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C137" s="10">
         <v>44477</v>
@@ -6786,10 +6786,10 @@
         <v>44827</v>
       </c>
       <c r="E137" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F137" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="F137" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="G137" s="11">
         <v>44827</v>
@@ -6820,9 +6820,9 @@
       <c r="AD137" s="8"/>
       <c r="AE137" s="8"/>
     </row>
-    <row r="138" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B138" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C138" s="10">
         <v>44471</v>
@@ -6831,10 +6831,10 @@
         <v>44828</v>
       </c>
       <c r="E138" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G138" s="11">
         <v>44828</v>
@@ -6846,11 +6846,11 @@
       <c r="J138" s="22"/>
       <c r="L138" s="8"/>
       <c r="M138" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N138" s="8"/>
       <c r="O138" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P138" s="8"/>
       <c r="Q138" s="8"/>
@@ -6869,17 +6869,17 @@
       <c r="AD138" s="8"/>
       <c r="AE138" s="8"/>
     </row>
-    <row r="139" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B139" s="9"/>
       <c r="C139" s="10"/>
       <c r="D139" s="11">
         <v>44828</v>
       </c>
       <c r="E139" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F139" s="45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G139" s="11">
         <v>44828</v>
@@ -6893,7 +6893,7 @@
       <c r="M139" s="8"/>
       <c r="N139" s="8"/>
       <c r="O139" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P139" s="8"/>
       <c r="Q139" s="8"/>
@@ -6912,17 +6912,17 @@
       <c r="AD139" s="8"/>
       <c r="AE139" s="8"/>
     </row>
-    <row r="140" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B140" s="9"/>
       <c r="C140" s="10"/>
       <c r="D140" s="11">
         <v>44828</v>
       </c>
       <c r="E140" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F140" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="F140" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="G140" s="11">
         <v>44828</v>
@@ -6951,9 +6951,9 @@
       <c r="AD140" s="8"/>
       <c r="AE140" s="8"/>
     </row>
-    <row r="141" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B141" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C141" s="10">
         <v>44472</v>
@@ -6962,10 +6962,10 @@
         <v>44829</v>
       </c>
       <c r="E141" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F141" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="F141" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="G141" s="11">
         <v>44829</v>
@@ -6994,17 +6994,17 @@
       <c r="AD141" s="8"/>
       <c r="AE141" s="8"/>
     </row>
-    <row r="142" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B142" s="9"/>
       <c r="C142" s="10"/>
       <c r="D142" s="11">
         <v>44829</v>
       </c>
       <c r="E142" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F142" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G142" s="11">
         <v>44829</v>
@@ -7033,14 +7033,14 @@
       <c r="AD142" s="8"/>
       <c r="AE142" s="8"/>
     </row>
-    <row r="143" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B143" s="9"/>
       <c r="C143" s="10"/>
       <c r="D143" s="11">
         <v>44829</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F143" s="13"/>
       <c r="G143" s="13"/>
@@ -7068,9 +7068,9 @@
       <c r="AD143" s="8"/>
       <c r="AE143" s="8"/>
     </row>
-    <row r="144" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B144" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C144" s="10">
         <v>44473</v>
@@ -7079,7 +7079,7 @@
         <v>44830</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F144" s="13"/>
       <c r="G144" s="13"/>
@@ -7107,9 +7107,9 @@
       <c r="AD144" s="8"/>
       <c r="AE144" s="8"/>
     </row>
-    <row r="145" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B145" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C145" s="10">
         <v>44474</v>
@@ -7118,10 +7118,10 @@
         <v>44831</v>
       </c>
       <c r="E145" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F145" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="F145" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G145" s="11">
         <v>44831</v>
@@ -7130,7 +7130,7 @@
       <c r="I145" s="21"/>
       <c r="J145" s="22"/>
       <c r="L145" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M145" s="8"/>
       <c r="N145" s="8"/>
@@ -7152,9 +7152,9 @@
       <c r="AD145" s="8"/>
       <c r="AE145" s="8"/>
     </row>
-    <row r="146" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B146" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C146" s="10">
         <v>44475</v>
@@ -7163,7 +7163,7 @@
         <v>44832</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F146" s="13"/>
       <c r="G146" s="13"/>
@@ -7191,9 +7191,9 @@
       <c r="AD146" s="8"/>
       <c r="AE146" s="8"/>
     </row>
-    <row r="147" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B147" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C147" s="10">
         <v>44476</v>
@@ -7202,10 +7202,10 @@
         <v>44833</v>
       </c>
       <c r="E147" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F147" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G147" s="11">
         <v>44833</v>
@@ -7214,7 +7214,7 @@
       <c r="I147" s="21"/>
       <c r="J147" s="22"/>
       <c r="L147" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M147" s="8"/>
       <c r="N147" s="8"/>
@@ -7236,9 +7236,9 @@
       <c r="AD147" s="8"/>
       <c r="AE147" s="8"/>
     </row>
-    <row r="148" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B148" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C148" s="10">
         <v>44477</v>
@@ -7247,10 +7247,10 @@
         <v>44834</v>
       </c>
       <c r="E148" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F148" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G148" s="11">
         <v>44834</v>
@@ -7279,9 +7279,9 @@
       <c r="AD148" s="8"/>
       <c r="AE148" s="8"/>
     </row>
-    <row r="149" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B149" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C149" s="47">
         <v>44473</v>
@@ -7290,7 +7290,7 @@
         <v>44837</v>
       </c>
       <c r="E149" s="49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F149" s="50"/>
       <c r="G149" s="50"/>
@@ -7318,7 +7318,7 @@
       <c r="AD149" s="8"/>
       <c r="AE149" s="8"/>
     </row>
-    <row r="150" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:31" x14ac:dyDescent="0.25">
       <c r="L150" s="1"/>
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>

</xml_diff>